<commit_message>
completed monitoring report calcs for 2021
</commit_message>
<xml_diff>
--- a/Data/MonitoringReport2021/2020ERMonitoredValuesSummary.xlsx
+++ b/Data/MonitoringReport2021/2020ERMonitoredValuesSummary.xlsx
@@ -8,8 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Monitoring Period Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Monitoring Report Parameters" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Monitoring Period Data'!$B$2:$H$21</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t xml:space="preserve">2019/2020 Monitoring Report Input Data</t>
   </si>
@@ -40,6 +44,9 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
+    <t xml:space="preserve">FRL Annual Average</t>
+  </si>
+  <si>
     <t xml:space="preserve">2019</t>
   </si>
   <si>
@@ -113,6 +120,9 @@
   </si>
   <si>
     <t xml:space="preserve">FPlnAreaHarvSwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Softwood Harvested Area</t>
   </si>
   <si>
     <t xml:space="preserve">Annual area harvested in Softwood plantations (ha)</t>
@@ -162,16 +172,96 @@
   </si>
   <si>
     <t xml:space="preserve">areaproportion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC Params</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC Runs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC Tolerance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitoring Period Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting Period Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest Reference Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRL Deforestation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRL Forest Degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRL Removals by Sinks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transferred Emission Reductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contested Emission Reductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sold Emission Reductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk Set Aside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative Previous Reference Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative Previous Emissions and Removals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative Previous Emission Reductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy Degradation Uncertainty Discount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -197,13 +287,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="20"/>
       <color rgb="FF000000"/>
@@ -227,8 +310,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +328,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -314,7 +409,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,42 +428,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,19 +473,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="5" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="6" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,23 +505,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="8" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="8" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="9" xfId="15" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal_S1-S4" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -447,7 +571,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -486,15 +610,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="B4:G14" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B4:G14"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="B4:H14" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B4:H14"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="RCode Name"/>
     <tableColumn id="2" name="Data Label"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="Source"/>
-    <tableColumn id="5" name="2019"/>
-    <tableColumn id="6" name="2020"/>
+    <tableColumn id="5" name="FRL Annual Average"/>
+    <tableColumn id="6" name="2019"/>
+    <tableColumn id="7" name="2020"/>
   </tableColumns>
 </table>
 </file>
@@ -502,24 +627,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B2:G21"/>
+  <dimension ref="B2:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,246 +670,585 @@
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="9" t="n">
+        <v>62199.5454545455</v>
+      </c>
+      <c r="G5" s="10" t="n">
         <v>19801.647</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="H5" s="11" t="n">
         <v>21441.157</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="9" t="n">
+        <v>56926</v>
+      </c>
+      <c r="G6" s="10" t="n">
         <v>40909.4</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="H6" s="11" t="n">
         <v>44813.46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="9" t="n">
+        <v>278</v>
+      </c>
+      <c r="G7" s="10" t="n">
         <v>4007.9</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="H7" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="9" t="n">
+        <v>301</v>
+      </c>
+      <c r="G8" s="10" t="n">
         <v>103.84</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="H8" s="11" t="n">
         <v>142.94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <v>334463.181818182</v>
+      </c>
+      <c r="G9" s="10" t="n">
         <v>386985</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="H9" s="11" t="n">
         <v>479959</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="F10" s="9" t="n">
+        <v>31141</v>
+      </c>
+      <c r="G10" s="10" t="n">
         <v>24698</v>
       </c>
-      <c r="G10" s="10" t="n">
+      <c r="H10" s="11" t="n">
         <v>26094</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="9" t="n">
+        <v>371</v>
+      </c>
+      <c r="G11" s="10" t="n">
         <v>2008</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="H11" s="11" t="n">
         <v>1910</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F12" s="9" t="n">
+        <v>1282</v>
+      </c>
+      <c r="G12" s="10" t="n">
         <v>909</v>
       </c>
-      <c r="G12" s="10" t="n">
+      <c r="H12" s="11" t="n">
         <v>1377</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="11" t="n">
+        <v>37</v>
+      </c>
+      <c r="F13" s="12" t="n">
+        <v>50731.4545454546</v>
+      </c>
+      <c r="G13" s="13" t="n">
         <v>27582.754</v>
       </c>
-      <c r="G13" s="12" t="n">
+      <c r="H13" s="14" t="n">
         <v>22088.296</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="C14" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="15" t="n">
+      <c r="D14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="17" t="n">
+        <v>1798.45454545455</v>
+      </c>
+      <c r="G14" s="18" t="n">
         <v>1349.88</v>
       </c>
-      <c r="G14" s="16" t="n">
+      <c r="H14" s="19" t="n">
         <v>1082.63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>45</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.0115</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0.0115</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>8121976</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>8121976</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>8121976</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>730</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>540</v>
+      </c>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="23" t="n">
+        <v>1874373</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="23" t="n">
+        <v>2548813.33</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="23" t="n">
+        <v>1101723.67</v>
+      </c>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="23" t="n">
+        <v>2696830</v>
+      </c>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="23" t="n">
+        <v>3252371.26</v>
+      </c>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="23" t="n">
+        <v>2048438.97</v>
+      </c>
+      <c r="C9" s="22"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="23" t="n">
+        <v>310442</v>
+      </c>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="23" t="n">
+        <v>381776.61</v>
+      </c>
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="23" t="n">
+        <v>241686.83</v>
+      </c>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="23" t="n">
+        <v>-1132900</v>
+      </c>
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="23" t="n">
+        <v>-751897.61</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>-1538544.58</v>
+      </c>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="22"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="22" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C19" s="22"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="22" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="C23" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -794,8 +1258,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>